<commit_message>
test random sphere packing bed, MR is a litte tricky
</commit_message>
<xml_diff>
--- a/Result/Sc/Sum_r.xlsx
+++ b/Result/Sc/Sum_r.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="9">
   <si>
     <t xml:space="preserve">Sbb-mrt</t>
   </si>
@@ -42,6 +43,12 @@
   </si>
   <si>
     <t xml:space="preserve">Ibm-mrtb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ibm-mrta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Psm-mrtb</t>
   </si>
 </sst>
 </file>
@@ -304,10 +311,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -340,6 +347,12 @@
       <c r="H1" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="I1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
@@ -363,6 +376,15 @@
       <c r="G2" s="1" t="n">
         <v>0.110132492</v>
       </c>
+      <c r="H2" s="1" t="n">
+        <v>0.129487491</v>
+      </c>
+      <c r="I2" s="1" t="n">
+        <v>0.123421751</v>
+      </c>
+      <c r="J2" s="1" t="n">
+        <v>0.0914734671</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
@@ -386,6 +408,15 @@
       <c r="G3" s="1" t="n">
         <v>0.0766529424</v>
       </c>
+      <c r="H3" s="1" t="n">
+        <v>0.0871822565</v>
+      </c>
+      <c r="I3" s="1" t="n">
+        <v>0.0888339192</v>
+      </c>
+      <c r="J3" s="1" t="n">
+        <v>0.0713024869</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
@@ -409,6 +440,15 @@
       <c r="G4" s="1" t="n">
         <v>0.0740130339</v>
       </c>
+      <c r="H4" s="1" t="n">
+        <v>0.0822136402</v>
+      </c>
+      <c r="I4" s="1" t="n">
+        <v>0.0827071371</v>
+      </c>
+      <c r="J4" s="1" t="n">
+        <v>0.0708284843</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
@@ -432,6 +472,15 @@
       <c r="G5" s="1" t="n">
         <v>0.0732646706</v>
       </c>
+      <c r="H5" s="1" t="n">
+        <v>0.0799363019</v>
+      </c>
+      <c r="I5" s="1" t="n">
+        <v>0.0800679722</v>
+      </c>
+      <c r="J5" s="1" t="n">
+        <v>0.0709763945</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
@@ -455,6 +504,15 @@
       <c r="G6" s="1" t="n">
         <v>0.0731095982</v>
       </c>
+      <c r="H6" s="1" t="n">
+        <v>0.0785600114</v>
+      </c>
+      <c r="I6" s="1" t="n">
+        <v>0.0785638005</v>
+      </c>
+      <c r="J6" s="1" t="n">
+        <v>0.0713362252</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
@@ -477,6 +535,89 @@
       </c>
       <c r="G7" s="1" t="n">
         <v>0.0728758522</v>
+      </c>
+      <c r="H7" s="1" t="n">
+        <v>0.0775220646</v>
+      </c>
+      <c r="I7" s="1" t="n">
+        <v>0.0774896726</v>
+      </c>
+      <c r="J7" s="1" t="n">
+        <v>0.0714295318</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:J7"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>